<commit_message>
Modifying py script to read in from excel file
</commit_message>
<xml_diff>
--- a/excercises.xlsx
+++ b/excercises.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e043f65062c432d7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiuns\Documents\analytics\workouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{E1F4A556-8C62-4A7B-90A6-BD44103C9220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CC4CFCA-8A91-4E77-9A2F-2FFF730FAFC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16594691-75F9-4AE4-A724-C28F8697B396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16DF580D-0C29-4318-BD3F-1925A8556864}"/>
+    <workbookView xWindow="5115" yWindow="4140" windowWidth="21600" windowHeight="11385" xr2:uid="{16DF580D-0C29-4318-BD3F-1925A8556864}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>Exercise</t>
   </si>
@@ -204,9 +204,6 @@
     <t>in push up position, bring knees to elbows and back</t>
   </si>
   <si>
-    <t>Australian push ups</t>
-  </si>
-  <si>
     <t>dead bugs</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>lie on back, point knees and hands to air, straighten one leg at a time</t>
   </si>
   <si>
-    <t>on hands and knees, extend one leg and opposing arm simultaneousle</t>
-  </si>
-  <si>
     <t>kickthroughs</t>
   </si>
   <si>
@@ -277,9 +271,6 @@
   </si>
   <si>
     <t>reverse plank/bridge</t>
-  </si>
-  <si>
-    <t>become a table with your stomack pointing to the sky; hold or just bring bum up and down</t>
   </si>
   <si>
     <t>can sit on the floor and "dip"; or use two chairs like a dip station;
@@ -306,6 +297,18 @@
   </si>
   <si>
     <t>lie on back, elbow to knee, then bring leg all the way up with your arm</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Australian pull ups</t>
+  </si>
+  <si>
+    <t>become a table with your stomach pointing to the sky; hold or just bring bum up and down</t>
+  </si>
+  <si>
+    <t>on hands and knees, extend one leg and opposing arm simultaneously</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10E6EC8-BF02-461E-906A-34C265DE6F41}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +676,7 @@
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,8 +686,11 @@
       <c r="C1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -692,7 +698,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -700,7 +706,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -708,7 +714,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -716,7 +722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -727,7 +733,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -738,7 +744,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -749,7 +755,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -757,7 +763,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -765,7 +771,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -773,7 +779,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -781,7 +787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -792,7 +798,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -800,7 +806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -808,7 +814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -987,171 +993,171 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" t="s">
         <v>69</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D50" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" t="s">
         <v>84</v>
-      </c>
-      <c r="D51" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D52" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix for shuffling that was having duplicate exercises per workout. tidying up exercises.xlsx file
</commit_message>
<xml_diff>
--- a/excercises.xlsx
+++ b/excercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiuns\Documents\analytics\workouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16594691-75F9-4AE4-A724-C28F8697B396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2703993-64BA-417D-9536-CCC2AD4F5B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="4140" windowWidth="21600" windowHeight="11385" xr2:uid="{16DF580D-0C29-4318-BD3F-1925A8556864}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16DF580D-0C29-4318-BD3F-1925A8556864}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
   <si>
     <t>Exercise</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>in plank position with feet apart, walk feet up to hands as far as possible, then back, keeping hands still</t>
-  </si>
-  <si>
-    <t>Use a chair</t>
   </si>
   <si>
     <t>reverse Incline push up</t>
@@ -283,10 +280,6 @@
     <t>to start, do a handstand, but with feet/knees on a chair</t>
   </si>
   <si>
-    <t>on stomach, lift up head and bring arms back like you're swimming a breast stroke;
-to make harder, lift up legs as well and swing arms to side</t>
-  </si>
-  <si>
     <t>crunches</t>
   </si>
   <si>
@@ -309,6 +302,15 @@
   </si>
   <si>
     <t>on hands and knees, extend one leg and opposing arm simultaneously</t>
+  </si>
+  <si>
+    <t>centr</t>
+  </si>
+  <si>
+    <t>pull up, use a chair or bar</t>
+  </si>
+  <si>
+    <t>on stomach, lift up head and bring arms back like you're swimming a breast stroke; to make harder, lift up legs as well and swing arms to side</t>
   </si>
 </sst>
 </file>
@@ -665,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10E6EC8-BF02-461E-906A-34C265DE6F41}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +689,7 @@
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -697,6 +699,9 @@
       <c r="C2" t="s">
         <v>41</v>
       </c>
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -705,6 +710,9 @@
       <c r="C3" t="s">
         <v>42</v>
       </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -713,6 +721,9 @@
       <c r="C4" t="s">
         <v>42</v>
       </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -721,6 +732,9 @@
       <c r="C5" t="s">
         <v>43</v>
       </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -732,6 +746,9 @@
       <c r="C6" t="s">
         <v>43</v>
       </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -743,6 +760,9 @@
       <c r="C7" t="s">
         <v>45</v>
       </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -754,6 +774,9 @@
       <c r="C8" t="s">
         <v>45</v>
       </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -762,6 +785,9 @@
       <c r="C9" t="s">
         <v>45</v>
       </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -770,6 +796,9 @@
       <c r="C10" t="s">
         <v>41</v>
       </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -778,6 +807,9 @@
       <c r="C11" t="s">
         <v>41</v>
       </c>
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -786,6 +818,9 @@
       <c r="C12" t="s">
         <v>41</v>
       </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -797,6 +832,9 @@
       <c r="C13" t="s">
         <v>45</v>
       </c>
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -805,6 +843,9 @@
       <c r="C14" t="s">
         <v>41</v>
       </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -813,6 +854,9 @@
       <c r="C15" t="s">
         <v>47</v>
       </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -821,16 +865,22 @@
       <c r="C16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -840,8 +890,11 @@
       <c r="C18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -851,104 +904,143 @@
       <c r="C19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="C29" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="C30" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
       <c r="C31" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -957,6 +1049,9 @@
       </c>
       <c r="C32" t="s">
         <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,6 +1061,9 @@
       <c r="C33" t="s">
         <v>41</v>
       </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -974,6 +1072,9 @@
       <c r="C34" t="s">
         <v>46</v>
       </c>
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -982,6 +1083,9 @@
       <c r="C35" t="s">
         <v>52</v>
       </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -990,13 +1094,16 @@
       <c r="C36" t="s">
         <v>46</v>
       </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" t="s">
-        <v>72</v>
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1012,7 +1119,7 @@
         <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1020,7 +1127,7 @@
         <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,76 +1195,76 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>76</v>
       </c>
-      <c r="D48" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>77</v>
-      </c>
       <c r="B49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" t="s">
         <v>82</v>
-      </c>
-      <c r="D49" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>